<commit_message>
Added in updated test case for VISA
</commit_message>
<xml_diff>
--- a/Test Cases/Splint 2 Test Cases.xlsx
+++ b/Test Cases/Splint 2 Test Cases.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6820" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="VISA" sheetId="1" r:id="rId1"/>
-    <sheet name="Medical" sheetId="2" r:id="rId2"/>
-    <sheet name="Top K Doctor" sheetId="3" r:id="rId3"/>
-    <sheet name="Top K Referral" sheetId="5" r:id="rId4"/>
-    <sheet name="Top K Specialty" sheetId="7" r:id="rId5"/>
-    <sheet name="Top K Specialty Result " sheetId="8" state="hidden" r:id="rId6"/>
-    <sheet name="Top K Referral Result" sheetId="6" state="hidden" r:id="rId7"/>
-    <sheet name="Top K Doctor Result" sheetId="4" state="hidden" r:id="rId8"/>
+    <sheet name="VISA(old)" sheetId="1" r:id="rId1"/>
+    <sheet name="VISA" sheetId="9" r:id="rId2"/>
+    <sheet name="Medical" sheetId="2" r:id="rId3"/>
+    <sheet name="Top K Doctor" sheetId="3" r:id="rId4"/>
+    <sheet name="Top K Referral" sheetId="5" r:id="rId5"/>
+    <sheet name="Top K Specialty" sheetId="7" r:id="rId6"/>
+    <sheet name="Top K Specialty Result " sheetId="8" state="hidden" r:id="rId7"/>
+    <sheet name="Top K Referral Result" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="Top K Doctor Result" sheetId="4" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Top K Doctor'!$I$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Top K Doctor Result'!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Top K Referral Result'!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Top K Specialty Result '!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Top K Doctor'!$I$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Top K Doctor Result'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Top K Referral Result'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Top K Specialty Result '!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="358">
   <si>
     <t xml:space="preserve">Month : August
 </t>
@@ -1278,6 +1279,26 @@
   </si>
   <si>
     <t>Actual Output</t>
+  </si>
+  <si>
+    <t>To compare the number of applications received</t>
+  </si>
+  <si>
+    <t>Australia Tourist : 5
+ICA STVP : 10 
+Indonesia - VKBKP 212 : 61
+Indonesia - VKU 211 : 50
+Indonesia - VTT 312 - Less than 6 months : 124
+Indonesia - VTT 312 - More than 6 months : 121
+Indonesia - VTT 316 - Less than 6 months: 1
+Indonesia - VTT 316 - More than 6 months: 2
+Indonesia - VTT 317 - Less than 6 months: 13
+Indonesia - VTT 317 - More than 6 months: 17
+Indonesia Entry Visa Extend : 1
+Maternity : 11</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1722,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1908,6 +1929,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="197" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
@@ -2330,7 +2407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
@@ -2599,11 +2676,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2753,7 +2830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2851,7 +2928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -3216,7 +3293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -3757,7 +3834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G209"/>
   <sheetViews>
@@ -6427,7 +6504,7 @@
         <v>1</v>
       </c>
       <c r="D194">
-        <f t="shared" ref="D194:D257" si="3">SUM(B194:C194)</f>
+        <f t="shared" ref="D194:D209" si="3">SUM(B194:C194)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>